<commit_message>
dbclickevent done, playlist fixing
</commit_message>
<xml_diff>
--- a/prototype_script.xlsx
+++ b/prototype_script.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\졸업작품\프로젝트\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klego\PycharmProjects\GraduationProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E1140D-5DB0-468E-B178-A0794B86CB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055F854D-9750-4538-BE89-39D938C926E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="-120" windowWidth="37530" windowHeight="16440" xr2:uid="{E26B7BC3-BCD6-4736-A66B-11DFB19A4BB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E26B7BC3-BCD6-4736-A66B-11DFB19A4BB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>내일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,46 +69,6 @@
   </si>
   <si>
     <t>검은색 정장 차림의 인도팀 사자들이 숙연한 표정으로 세 갈래의 골목길에서 나와 영천의 집으로 줄지어 오고 있다.</t>
-  </si>
-  <si>
-    <t>2초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>27초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>41초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>44초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>52초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">77초 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>90초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -483,97 +443,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F46A89-5862-4201-90B7-FB2436102335}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
-      </c>
-      <c r="L11" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>